<commit_message>
Carga indicador 3 - Empleo
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3F20B9-01D7-42BB-8C66-31E6E8380EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD50906D-98CD-4FDA-9E1C-0AC8CB262F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Indicador</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Indicador 10</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Salario</t>
+  </si>
+  <si>
+    <t>CoL</t>
   </si>
 </sst>
 </file>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,11 +452,12 @@
     <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,76 +477,151 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C2">
+        <v>1999</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2">
+        <v>2021</v>
+      </c>
+      <c r="F2">
+        <v>2031</v>
+      </c>
+      <c r="G2">
+        <v>1999</v>
+      </c>
+      <c r="H2">
+        <v>2031</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="C3">
+        <v>2011</v>
+      </c>
+      <c r="D3">
+        <v>2050</v>
+      </c>
+      <c r="G3">
+        <v>2011</v>
+      </c>
+      <c r="H3">
+        <v>2031</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>2002</v>
+      </c>
+      <c r="D4">
+        <v>2022</v>
+      </c>
+      <c r="E4">
+        <v>2023</v>
+      </c>
+      <c r="F4">
+        <v>2031</v>
+      </c>
+      <c r="G4">
+        <v>2002</v>
+      </c>
+      <c r="H4">
+        <v>2031</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Limpieza indicadores 7 y 8
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783256B-07F8-47FF-8215-E5D81B953B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF3D50-1D63-4394-9870-B64CE7F230B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Indicador</t>
   </si>
@@ -121,6 +132,12 @@
   </si>
   <si>
     <t>Esperanza vida</t>
+  </si>
+  <si>
+    <t>Crímenes</t>
+  </si>
+  <si>
+    <t>Servicios</t>
   </si>
 </sst>
 </file>
@@ -456,7 +473,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,15 +718,111 @@
       <c r="B7" t="s">
         <v>31</v>
       </c>
+      <c r="C7">
+        <v>1993</v>
+      </c>
+      <c r="D7">
+        <v>2018</v>
+      </c>
+      <c r="E7">
+        <v>2019</v>
+      </c>
+      <c r="F7">
+        <v>2031</v>
+      </c>
+      <c r="G7">
+        <v>1993</v>
+      </c>
+      <c r="H7">
+        <v>2031</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>2010</v>
+      </c>
+      <c r="D8">
+        <v>2022</v>
+      </c>
+      <c r="E8">
+        <v>2023</v>
+      </c>
+      <c r="F8">
+        <v>2031</v>
+      </c>
+      <c r="G8">
+        <v>2010</v>
+      </c>
+      <c r="H8">
+        <v>2031</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>2009</v>
+      </c>
+      <c r="D9">
+        <v>2024</v>
+      </c>
+      <c r="E9">
+        <v>2025</v>
+      </c>
+      <c r="F9">
+        <v>2031</v>
+      </c>
+      <c r="G9">
+        <v>2009</v>
+      </c>
+      <c r="H9">
+        <v>2031</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Actualización limpieza indicador 1
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF04083D-205F-4058-B01D-FB071012DFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B4A16B-83F9-4949-9142-26F3F9F97F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36495" yWindow="4140" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,10 +566,10 @@
         <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modificaciones limpieza indicador 2
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B4A16B-83F9-4949-9142-26F3F9F97F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206DAB78-175B-434F-93F5-EE7F5C8B5179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36495" yWindow="4140" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,7 +601,7 @@
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Actualización limpieza indicador 3
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206DAB78-175B-434F-93F5-EE7F5C8B5179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14C484A-0800-48E2-828C-CC676526007C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36495" yWindow="4140" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Indicador 3 - OK
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14C484A-0800-48E2-828C-CC676526007C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4F9141-36E1-415B-BBEB-02CDCEDAC643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36495" yWindow="4140" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Indicador</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Alquiler</t>
+  </si>
+  <si>
+    <t>Actualizar con datos desde 2001</t>
   </si>
 </sst>
 </file>
@@ -477,64 +480,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.109375" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.44140625" customWidth="1"/>
+    <col min="16" max="16" width="1.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -545,22 +553,22 @@
         <v>1999</v>
       </c>
       <c r="D2">
+        <v>1999</v>
+      </c>
+      <c r="E2">
         <v>2020</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2021</v>
       </c>
-      <c r="F2">
-        <v>2031</v>
-      </c>
       <c r="G2">
+        <v>2031</v>
+      </c>
+      <c r="H2">
         <v>1999</v>
       </c>
-      <c r="H2">
-        <v>2031</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
+      <c r="I2">
+        <v>2031</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
@@ -569,10 +577,16 @@
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -580,31 +594,40 @@
         <v>11</v>
       </c>
       <c r="C3">
+        <v>2001</v>
+      </c>
+      <c r="D3">
         <v>2011</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2050</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2011</v>
       </c>
-      <c r="H3">
-        <v>2031</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>2031</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -615,34 +638,40 @@
         <v>2002</v>
       </c>
       <c r="D4">
+        <v>2002</v>
+      </c>
+      <c r="E4">
         <v>2022</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2023</v>
       </c>
-      <c r="F4">
-        <v>2031</v>
-      </c>
       <c r="G4">
+        <v>2031</v>
+      </c>
+      <c r="H4">
         <v>2002</v>
       </c>
-      <c r="H4">
-        <v>2031</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
+      <c r="I4">
+        <v>2031</v>
       </c>
       <c r="J4" t="s">
         <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -653,34 +682,40 @@
         <v>2004</v>
       </c>
       <c r="D5">
+        <v>2004</v>
+      </c>
+      <c r="E5">
         <v>2021</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2022</v>
       </c>
-      <c r="F5">
-        <v>2031</v>
-      </c>
       <c r="G5">
+        <v>2031</v>
+      </c>
+      <c r="H5">
         <v>2004</v>
       </c>
-      <c r="H5">
-        <v>2031</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
+      <c r="I5">
+        <v>2031</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>
       </c>
       <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
         <v>29</v>
       </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -691,22 +726,22 @@
         <v>1993</v>
       </c>
       <c r="D6">
+        <v>1993</v>
+      </c>
+      <c r="E6">
         <v>2023</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2024</v>
       </c>
-      <c r="F6">
-        <v>2031</v>
-      </c>
       <c r="G6">
+        <v>2031</v>
+      </c>
+      <c r="H6">
         <v>1993</v>
       </c>
-      <c r="H6">
-        <v>2031</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
+      <c r="I6">
+        <v>2031</v>
       </c>
       <c r="J6" t="s">
         <v>12</v>
@@ -715,48 +750,54 @@
         <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7">
+      <c r="D7">
+        <v>2003</v>
+      </c>
+      <c r="E7">
+        <v>2022</v>
+      </c>
+      <c r="F7">
+        <v>2019</v>
+      </c>
+      <c r="G7">
+        <v>2031</v>
+      </c>
+      <c r="H7">
         <v>1993</v>
       </c>
-      <c r="D7">
-        <v>2018</v>
-      </c>
-      <c r="E7">
-        <v>2019</v>
-      </c>
-      <c r="F7">
-        <v>2031</v>
-      </c>
-      <c r="G7">
-        <v>1993</v>
-      </c>
-      <c r="H7">
-        <v>2031</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
+      <c r="I7">
+        <v>2031</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -764,37 +805,43 @@
         <v>32</v>
       </c>
       <c r="C8">
+        <v>1999</v>
+      </c>
+      <c r="D8">
         <v>2010</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>2022</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2023</v>
       </c>
-      <c r="F8">
-        <v>2031</v>
-      </c>
       <c r="G8">
+        <v>2031</v>
+      </c>
+      <c r="H8">
         <v>2010</v>
       </c>
-      <c r="H8">
-        <v>2031</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="I8">
+        <v>2031</v>
+      </c>
+      <c r="J8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
       <c r="K8" t="s">
         <v>14</v>
       </c>
       <c r="L8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -802,25 +849,25 @@
         <v>33</v>
       </c>
       <c r="C9">
+        <v>2003</v>
+      </c>
+      <c r="D9">
         <v>2009</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2024</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2025</v>
       </c>
-      <c r="F9">
-        <v>2031</v>
-      </c>
       <c r="G9">
+        <v>2031</v>
+      </c>
+      <c r="H9">
         <v>2009</v>
       </c>
-      <c r="H9">
-        <v>2031</v>
-      </c>
-      <c r="I9" t="s">
-        <v>12</v>
+      <c r="I9">
+        <v>2031</v>
       </c>
       <c r="J9" t="s">
         <v>12</v>
@@ -829,10 +876,16 @@
         <v>12</v>
       </c>
       <c r="L9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="M9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -843,22 +896,22 @@
         <v>1995</v>
       </c>
       <c r="D10">
-        <v>2017</v>
+        <v>1995</v>
       </c>
       <c r="E10">
+        <v>2024</v>
+      </c>
+      <c r="F10">
         <v>2018</v>
       </c>
-      <c r="F10">
-        <v>2031</v>
-      </c>
       <c r="G10">
+        <v>2031</v>
+      </c>
+      <c r="H10">
         <v>1995</v>
       </c>
-      <c r="H10">
-        <v>2031</v>
-      </c>
-      <c r="I10" t="s">
-        <v>12</v>
+      <c r="I10">
+        <v>2031</v>
       </c>
       <c r="J10" t="s">
         <v>12</v>
@@ -867,45 +920,54 @@
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1997</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>2023</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2024</v>
       </c>
-      <c r="F11">
-        <v>2031</v>
-      </c>
       <c r="G11">
+        <v>2031</v>
+      </c>
+      <c r="H11">
         <v>1997</v>
       </c>
-      <c r="H11">
-        <v>2031</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="I11">
+        <v>2031</v>
+      </c>
+      <c r="J11" t="s">
         <v>13</v>
       </c>
-      <c r="J11" t="s">
-        <v>12</v>
-      </c>
       <c r="K11" t="s">
         <v>12</v>
       </c>
       <c r="L11" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indicadores 5 y 9 - OK
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4F9141-36E1-415B-BBEB-02CDCEDAC643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B06A51-D938-4659-B9C6-0A4D128660DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Indicador</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Actualizar con datos desde 2001</t>
+  </si>
+  <si>
+    <t>Fusionar los datos de 1999 antes de estimar</t>
   </si>
 </sst>
 </file>
@@ -177,12 +180,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -197,9 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +507,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +567,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -587,7 +611,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
@@ -628,7 +652,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
@@ -672,7 +696,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
@@ -716,7 +740,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -760,7 +784,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -798,7 +822,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
@@ -837,12 +861,15 @@
       <c r="M8" t="s">
         <v>14</v>
       </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
       <c r="Q8">
         <v>2022</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
@@ -886,7 +913,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
@@ -930,7 +957,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">

</xml_diff>

<commit_message>
Limpieza indicador 10 - OK
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B06A51-D938-4659-B9C6-0A4D128660DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C669F59-185D-4A41-82F2-83DB3209BC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -957,7 +957,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">

</xml_diff>

<commit_message>
Limpieza indicador 8 - OK
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C669F59-185D-4A41-82F2-83DB3209BC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4183160-02A2-4E9A-94BC-85997524E5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +869,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">

</xml_diff>

<commit_message>
Limpieza indicador 6 - OK
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4183160-02A2-4E9A-94BC-85997524E5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056B74B4-EAC2-4A0E-B891-4A75E4169FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,12 +218,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +510,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +787,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -820,6 +823,7 @@
       <c r="M7" t="s">
         <v>14</v>
       </c>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">

</xml_diff>

<commit_message>
Visor indicadores en tableau
</commit_message>
<xml_diff>
--- a/Estado_Indicadores.xlsx
+++ b/Estado_Indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formación\UOC\Asignaturas\12 - TFM\M3\UOC_TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA5AFF4-5691-4107-BCBE-6961D7834732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B842E850-90AC-4D2A-9C55-F2F79C1FE96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="156">
   <si>
     <t>Indicador</t>
   </si>
@@ -497,6 +497,15 @@
   </si>
   <si>
     <t>Aloja algunos de los edificios más altos en Londres en la zona denominada Canary Wharf, una parte del Queen Elizabeth Olympic Park, es uno de los mayores distritos financieros del país</t>
+  </si>
+  <si>
+    <t>Sede de las olimpiadas con Lee Valley Hockey and Tennis Centre and part of the Queen Elizabeth Olympic Park</t>
+  </si>
+  <si>
+    <t>Sede del nuevo mercado de Covent Garden y el Helipuerto de Londres</t>
+  </si>
+  <si>
+    <t>Lugares emblemáticos como el Parlamento, El British government, zona de compras Oxford Street, Regent Street, Picacadilly, Bond Street, Soho, Buckingham Palace, Westminster Abbey, WhiteHall, Trafalgar Square, Hyde Park, gran parte de Regent's Park</t>
   </si>
 </sst>
 </file>
@@ -848,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -1314,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C143DD9-00C5-40C7-9E8B-5539DA3CA130}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1912,6 +1921,18 @@
       <c r="B31" t="s">
         <v>96</v>
       </c>
+      <c r="C31">
+        <v>38.82</v>
+      </c>
+      <c r="D31">
+        <v>1965</v>
+      </c>
+      <c r="E31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1920,16 +1941,34 @@
       <c r="B32" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>34.26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>99</v>
       </c>
       <c r="B33" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>21.48</v>
+      </c>
+      <c r="E33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>101</v>
       </c>

</xml_diff>